<commit_message>
issue/#55 fix IndexError: list index out of range | change data supplier excel(contact person)
</commit_message>
<xml_diff>
--- a/Import_File_Test/suppliersData.xlsx
+++ b/Import_File_Test/suppliersData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="23110" windowHeight="12940"/>
+    <workbookView windowWidth="25520" windowHeight="12940"/>
   </bookViews>
   <sheets>
     <sheet name="Suppliers" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <t>電話</t>
   </si>
   <si>
-    <t>連絡人名稱</t>
+    <t>連絡人</t>
   </si>
   <si>
     <t>Email</t>
@@ -79,12 +79,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,9 +99,52 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <name val="新細明體"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="新細明體"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -114,54 +157,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="新細明體"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -183,25 +181,18 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="新細明體"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -227,6 +218,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -235,16 +233,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -259,31 +265,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -295,151 +427,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -464,21 +470,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -507,6 +498,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -518,11 +524,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -542,15 +546,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -565,124 +560,150 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -691,34 +712,22 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1063,7 +1072,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="6"/>
@@ -1078,7 +1087,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1104,7 +1113,7 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E2">
@@ -1127,7 +1136,7 @@
       <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E3">

</xml_diff>